<commit_message>
with input and tree output
</commit_message>
<xml_diff>
--- a/Junction_Info.xlsx
+++ b/Junction_Info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limor\PycharmProjects\smartJunction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87ED18DD-5BEE-409F-9449-67F25B7EB28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C114A5-426E-407C-BF00-5B28C0D8904D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2E427FA-550A-46C0-815F-1B170FDD5BC9}"/>
   </bookViews>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>number_of_lanes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>west</t>
   </si>
@@ -55,22 +49,34 @@
     <t>east</t>
   </si>
   <si>
+    <t>numOfLanes</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>junction name</t>
+  </si>
+  <si>
+    <t>ease</t>
+  </si>
+  <si>
+    <t>Morasha</t>
+  </si>
+  <si>
+    <t>Yarkon</t>
+  </si>
+  <si>
+    <t>BarIlan</t>
+  </si>
+  <si>
+    <t>AlufSafe</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
   </si>
 </sst>
 </file>
@@ -426,21 +432,31 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.796875" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="18.796875" customWidth="1"/>
     <col min="3" max="3" width="20.296875" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="17.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="17.69921875" customWidth="1"/>
+    <col min="9" max="9" width="16.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1">
         <v>1</v>
@@ -460,22 +476,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -483,22 +499,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -506,19 +522,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -526,7 +545,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -535,13 +554,13 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -552,16 +571,19 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -571,20 +593,17 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all classes, fetch from files needed
</commit_message>
<xml_diff>
--- a/Junction_Info.xlsx
+++ b/Junction_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limor\PycharmProjects\smartJunction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7C2612-699F-4552-93D7-EBC857AD52BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92221B4E-82EC-4C10-B3CD-0F9F39CB1586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2E427FA-550A-46C0-815F-1B170FDD5BC9}"/>
   </bookViews>
@@ -35,42 +35,150 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
-  <si>
-    <t>junction name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>Num_of_traffic_lights</t>
-  </si>
-  <si>
-    <t>Num_of_oprions</t>
-  </si>
-  <si>
-    <t>red_time</t>
-  </si>
-  <si>
-    <t>green_time</t>
-  </si>
-  <si>
-    <t>traffic_light_name</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>options</t>
-  </si>
-  <si>
-    <t>straight:south, left:west</t>
-  </si>
-  <si>
-    <t>left:east</t>
-  </si>
-  <si>
-    <t>right:east</t>
+    <t>JunctionName</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>right="south"</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>right="west", straight="south"</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>right="east", straight="north"</t>
+  </si>
+  <si>
+    <t>right="north", straight="west"</t>
+  </si>
+  <si>
+    <t>left="south"</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>right="north", left="south"</t>
+  </si>
+  <si>
+    <t>left="east", straight="south"</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>right="east", left="west"</t>
+  </si>
+  <si>
+    <t>right="south", straight="west"</t>
+  </si>
+  <si>
+    <t>left="south", straight="east"</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>right="north", straight="east"</t>
+  </si>
+  <si>
+    <t>traffic_light1</t>
+  </si>
+  <si>
+    <t>traffic_light1_sign</t>
+  </si>
+  <si>
+    <t>traffic_light2</t>
+  </si>
+  <si>
+    <t>traffic_light2_sign</t>
+  </si>
+  <si>
+    <t>traffic_light3_sign</t>
+  </si>
+  <si>
+    <t>traffic_light3</t>
+  </si>
+  <si>
+    <t>number_of_traffic_lights</t>
+  </si>
+  <si>
+    <t>south</t>
+  </si>
+  <si>
+    <t>east</t>
+  </si>
+  <si>
+    <t>west</t>
+  </si>
+  <si>
+    <t>north</t>
+  </si>
+  <si>
+    <t>junction_path</t>
+  </si>
+  <si>
+    <t>right=east, straight=north</t>
   </si>
 </sst>
 </file>
@@ -430,126 +538,333 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BED8FA2-09DD-4E6D-96F7-9186AB385D84}">
-  <dimension ref="B1:M4"/>
+  <dimension ref="B1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.19921875" customWidth="1"/>
-    <col min="2" max="2" width="18.796875" customWidth="1"/>
+    <col min="2" max="2" width="14.296875" customWidth="1"/>
     <col min="3" max="3" width="20.296875" customWidth="1"/>
-    <col min="4" max="4" width="15.796875" customWidth="1"/>
-    <col min="5" max="5" width="17.3984375" customWidth="1"/>
-    <col min="6" max="6" width="12.3984375" customWidth="1"/>
-    <col min="7" max="7" width="14.296875" customWidth="1"/>
-    <col min="8" max="8" width="19.8984375" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="24.8984375" customWidth="1"/>
+    <col min="7" max="7" width="24.59765625" customWidth="1"/>
+    <col min="8" max="8" width="26.09765625" customWidth="1"/>
     <col min="9" max="9" width="16.59765625" customWidth="1"/>
-    <col min="10" max="10" width="14.8984375" customWidth="1"/>
+    <col min="10" max="10" width="19.796875" customWidth="1"/>
     <col min="12" max="12" width="10.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="H4" s="1"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
simulation for number of users
</commit_message>
<xml_diff>
--- a/Junction_Info.xlsx
+++ b/Junction_Info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limor\PycharmProjects\smartJunction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92221B4E-82EC-4C10-B3CD-0F9F39CB1586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C1153C-9BFD-44F8-A569-EEF121198E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2E427FA-550A-46C0-815F-1B170FDD5BC9}"/>
   </bookViews>

</xml_diff>

<commit_message>
finished junction input. saved in list_of_junctions variable
</commit_message>
<xml_diff>
--- a/Junction_Info.xlsx
+++ b/Junction_Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limor\PycharmProjects\smartJunction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs File HDD\PycharmProjects\smart_Junction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92221B4E-82EC-4C10-B3CD-0F9F39CB1586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2031765-1DA6-4100-B313-3A0E62056121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2E427FA-550A-46C0-815F-1B170FDD5BC9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E2E427FA-550A-46C0-815F-1B170FDD5BC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
   <si>
     <t>A</t>
   </si>
@@ -154,12 +154,6 @@
     <t>traffic_light2_sign</t>
   </si>
   <si>
-    <t>traffic_light3_sign</t>
-  </si>
-  <si>
-    <t>traffic_light3</t>
-  </si>
-  <si>
     <t>number_of_traffic_lights</t>
   </si>
   <si>
@@ -179,26 +173,32 @@
   </si>
   <si>
     <t>right=east, straight=north</t>
+  </si>
+  <si>
+    <t>traffic_light1_redTimer,GreenTimer</t>
+  </si>
+  <si>
+    <t>100,1</t>
+  </si>
+  <si>
+    <t>traffic_light2_redTimer,GreenTimer</t>
+  </si>
+  <si>
+    <t>number_of_junction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,9 +221,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -242,7 +241,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -538,36 +537,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BED8FA2-09DD-4E6D-96F7-9186AB385D84}">
-  <dimension ref="B1:J22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.19921875" customWidth="1"/>
-    <col min="2" max="2" width="14.296875" customWidth="1"/>
-    <col min="3" max="3" width="20.296875" customWidth="1"/>
-    <col min="4" max="4" width="20.3984375" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
-    <col min="6" max="6" width="24.8984375" customWidth="1"/>
-    <col min="7" max="7" width="24.59765625" customWidth="1"/>
-    <col min="8" max="8" width="26.09765625" customWidth="1"/>
-    <col min="9" max="9" width="16.59765625" customWidth="1"/>
-    <col min="10" max="10" width="19.796875" customWidth="1"/>
-    <col min="12" max="12" width="10.19921875" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
@@ -576,19 +578,22 @@
         <v>36</v>
       </c>
       <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
-        <v>40</v>
-      </c>
       <c r="J1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -596,27 +601,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -625,19 +632,24 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -646,18 +658,24 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -665,8 +683,11 @@
       <c r="F6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -674,12 +695,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -687,13 +708,16 @@
       <c r="F8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -701,13 +725,16 @@
       <c r="F9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -715,8 +742,11 @@
       <c r="F10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -724,12 +754,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
@@ -737,13 +767,16 @@
       <c r="F12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
         <v>21</v>
@@ -751,13 +784,16 @@
       <c r="F13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
@@ -765,8 +801,11 @@
       <c r="F14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -774,12 +813,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
         <v>26</v>
@@ -787,13 +826,16 @@
       <c r="F16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
@@ -801,13 +843,16 @@
       <c r="F17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
         <v>24</v>
@@ -815,8 +860,11 @@
       <c r="F18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -824,12 +872,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
         <v>32</v>
@@ -837,13 +885,16 @@
       <c r="F20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
         <v>31</v>
@@ -851,19 +902,25 @@
       <c r="F21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
       </c>
       <c r="F22" t="s">
         <v>27</v>
+      </c>
+      <c r="G22" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>